<commit_message>
Rev B build release
git-svn-id: http://svn:8000/svn/INDEX/trunk@103 71e9ff3b-2aa0-ee42-b4dd-db5a0b4f3664
</commit_message>
<xml_diff>
--- a/hw/scanner/schematic/scanner_revB.xlsx
+++ b/hw/scanner/schematic/scanner_revB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="SCANNER_revb_1" localSheetId="0">Sheet1!$A$1:$L$99</definedName>
+    <definedName name="SCANNER_revb" localSheetId="0">Sheet1!$A$1:$L$103</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -31,12 +31,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="256">
-  <si>
-    <t>Top Level  Revised: Monday, May 16, 2016</t>
-  </si>
-  <si>
-    <t>Index Scanner          Revision: J</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="273">
+  <si>
+    <t>Top Level  Revised: Tuesday, May 31, 2016</t>
+  </si>
+  <si>
+    <t>Index Scanner Iss 2          Revision: B</t>
   </si>
   <si>
     <t>Fen Technology Ltd</t>
@@ -54,6 +54,9 @@
     <t>CB24 3DQ</t>
   </si>
   <si>
+    <t>Bill Of Materials           June 5,2016      17:37:55</t>
+  </si>
+  <si>
     <t>Page1</t>
   </si>
   <si>
@@ -141,7 +144,7 @@
     <t>C48,C52,C53,C54,C56,C57,</t>
   </si>
   <si>
-    <t>C59,C63,C66,C69</t>
+    <t>C59,C60,C63,C66,C69</t>
   </si>
   <si>
     <t>C17</t>
@@ -213,7 +216,7 @@
     <t>BLUE</t>
   </si>
   <si>
-    <t>Wurth_150141BS73100</t>
+    <t>LED_WURTH_WL-SMTW-150141BS73100</t>
   </si>
   <si>
     <t>Wurth</t>
@@ -228,7 +231,7 @@
     <t>WE-150141RV73100</t>
   </si>
   <si>
-    <t>Wurth_150141RV73100</t>
+    <t>LED_WURTH_WL-SBTW-150141RV73100</t>
   </si>
   <si>
     <t>150141RV73100</t>
@@ -255,19 +258,16 @@
     <t>J1</t>
   </si>
   <si>
-    <t>FTSH-105-01-F-DV-K</t>
-  </si>
-  <si>
-    <t>CON_10W_DV_SM_FTSH</t>
-  </si>
-  <si>
-    <t>Samtec</t>
-  </si>
-  <si>
-    <t>Digikey</t>
-  </si>
-  <si>
-    <t>SAM8796-ND</t>
+    <t>TC2050_IDC</t>
+  </si>
+  <si>
+    <t>TC2050IDC-NL</t>
+  </si>
+  <si>
+    <t>Tag_connect</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
   <si>
     <t>J2</t>
@@ -276,7 +276,7 @@
     <t>Molex 12W FFC 0.5mm</t>
   </si>
   <si>
-    <t>molex_52746-1271</t>
+    <t>CONN_MOLEX_52746-12WAY</t>
   </si>
   <si>
     <t>Molex</t>
@@ -288,7 +288,7 @@
     <t>J3</t>
   </si>
   <si>
-    <t>molex_1054431101</t>
+    <t>CONN_USB-AB_MOLEXWP_SD105443-110_0.65P</t>
   </si>
   <si>
     <t>J4</t>
@@ -297,7 +297,7 @@
     <t>53261-0371</t>
   </si>
   <si>
-    <t>53261-3way</t>
+    <t>CONN_MOLEX_53261-3WAY_RA</t>
   </si>
   <si>
     <t>L1</t>
@@ -321,18 +321,24 @@
     <t>3.3uH/0.65A</t>
   </si>
   <si>
+    <t>IND_744030003</t>
+  </si>
+  <si>
     <t>L8</t>
   </si>
   <si>
     <t>3.3uH/2A</t>
   </si>
   <si>
+    <t>IND_COILCRAFT_LPS4018_3.9X3.9_1.8H</t>
+  </si>
+  <si>
+    <t>Coilcraft</t>
+  </si>
+  <si>
     <t>LPS4018-332MRC</t>
   </si>
   <si>
-    <t>Coilcraft</t>
-  </si>
-  <si>
     <t>Mouser</t>
   </si>
   <si>
@@ -345,7 +351,7 @@
     <t>FDC6420</t>
   </si>
   <si>
-    <t>SuperSOT6</t>
+    <t>SOT23-6L</t>
   </si>
   <si>
     <t>Fairchild</t>
@@ -366,7 +372,7 @@
     <t>IRLML0030TRPBF</t>
   </si>
   <si>
-    <t>SOT23</t>
+    <t>SOT23-132</t>
   </si>
   <si>
     <t>IR</t>
@@ -378,21 +384,24 @@
     <t>BC857C</t>
   </si>
   <si>
-    <t>SOT-23</t>
-  </si>
-  <si>
     <t>NXP</t>
   </si>
   <si>
     <t>Q4,Q5,Q6,Q7,Q8,Q9,Q10</t>
   </si>
   <si>
-    <t>BC847BS</t>
+    <t>MUN5211DW</t>
   </si>
   <si>
     <t>SOT363</t>
   </si>
   <si>
+    <t>On Semi</t>
+  </si>
+  <si>
+    <t>MUN5211DW1T1G</t>
+  </si>
+  <si>
     <t>R1</t>
   </si>
   <si>
@@ -402,43 +411,40 @@
     <t>RC0603JR-0715RL</t>
   </si>
   <si>
-    <t>R2,R6,R8,R10,R16,R18,R19,</t>
+    <t>R3,R5,R15,R35,R75,R79,</t>
+  </si>
+  <si>
+    <t>100K</t>
+  </si>
+  <si>
+    <t>Multicomp</t>
+  </si>
+  <si>
+    <t>MC 0.0625W 0402 1% 100K</t>
+  </si>
+  <si>
+    <t>R80,R82,R102,R106,R107</t>
+  </si>
+  <si>
+    <t>R6,R8,R10,R16,R18,R19,</t>
   </si>
   <si>
     <t>10K</t>
   </si>
   <si>
-    <t>Multicomp</t>
-  </si>
-  <si>
     <t>MC 0.0625W 0402 1% 10K</t>
   </si>
   <si>
-    <t>R21,R22,R23,R24,R30,R40,</t>
-  </si>
-  <si>
-    <t>R43,R44,R45,R46,R49,R59,</t>
-  </si>
-  <si>
-    <t>R78,R83,R84,R86,R87,R88,</t>
-  </si>
-  <si>
-    <t>R89,R91,R92,R93,R94,R95,</t>
-  </si>
-  <si>
-    <t>R96,R101,R104,R105,R110</t>
-  </si>
-  <si>
-    <t>R3,R5,R15,R35,R75,R79,</t>
-  </si>
-  <si>
-    <t>100K</t>
-  </si>
-  <si>
-    <t>MC 0.0625W 0402 1% 100K</t>
-  </si>
-  <si>
-    <t>R80,R82,R102,R106,R107</t>
+    <t>R21,R22,R23,R24,R26,R29,</t>
+  </si>
+  <si>
+    <t>R30,R40,R43,R44,R45,R46,</t>
+  </si>
+  <si>
+    <t>R49,R59,R78,R101,R104,</t>
+  </si>
+  <si>
+    <t>R105,R110</t>
   </si>
   <si>
     <t>R11,R12</t>
@@ -477,6 +483,18 @@
     <t>MC 0.0625W 0402 1% 22R</t>
   </si>
   <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>0.01R</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>WSL0603R0100FEA</t>
+  </si>
+  <si>
     <t>R31,R32,R99,R100,R108</t>
   </si>
   <si>
@@ -486,6 +504,9 @@
     <t>MC 0.0625W 0402 1% 15K</t>
   </si>
   <si>
+    <t>R33,R39,R50</t>
+  </si>
+  <si>
     <t>DNF</t>
   </si>
   <si>
@@ -591,24 +612,27 @@
     <t>MCDHN-02F-V</t>
   </si>
   <si>
+    <t>SW_MULTICOMP_MCDHN_2WAY_3.8X4.5</t>
+  </si>
+  <si>
     <t>S1,S2</t>
   </si>
   <si>
     <t>SKRAALE010</t>
   </si>
   <si>
+    <t>SW_ALPS_SKRAALE010_6.2X6.2_3.4H</t>
+  </si>
+  <si>
     <t>ALPS</t>
   </si>
   <si>
-    <t>TPVIA2,TPVIA3,TPVIA4,</t>
+    <t>TPVIA2,TPVIA6,TPVIA7,</t>
   </si>
   <si>
     <t>TPVIA</t>
   </si>
   <si>
-    <t>TPVIA5,TPVIA6,TPVIA7,</t>
-  </si>
-  <si>
     <t>TPVIA8,TPVIA9,TPVIA10,</t>
   </si>
   <si>
@@ -636,12 +660,33 @@
     <t>TPVIA32,TPVIA33,TPVIA34</t>
   </si>
   <si>
+    <t>TP1,TP2,TP3,TP4,TP5,TP6,</t>
+  </si>
+  <si>
+    <t>TP_DFM_NOFILL</t>
+  </si>
+  <si>
+    <t>TP_DFM</t>
+  </si>
+  <si>
+    <t>TP7,TP8,TP9,TP10,TP11,</t>
+  </si>
+  <si>
+    <t>TP12,TP13,TP14,TP15,TP16,</t>
+  </si>
+  <si>
+    <t>TP17</t>
+  </si>
+  <si>
     <t>U1</t>
   </si>
   <si>
     <t>BTM805CL2B</t>
   </si>
   <si>
+    <t>MODULE_FLAIRCOMM-FLCBTM805</t>
+  </si>
+  <si>
     <t>FlairMicro</t>
   </si>
   <si>
@@ -672,9 +717,6 @@
     <t>STM809RWX6F</t>
   </si>
   <si>
-    <t>SOT23-3</t>
-  </si>
-  <si>
     <t>ST Microelectronics</t>
   </si>
   <si>
@@ -696,7 +738,7 @@
     <t>SN74LVC1G74DCU</t>
   </si>
   <si>
-    <t>8VSSOP</t>
+    <t>SO8_2.0X2.4_0.5</t>
   </si>
   <si>
     <t>TI</t>
@@ -720,16 +762,13 @@
     <t>U7</t>
   </si>
   <si>
-    <t>SOT23-6L</t>
-  </si>
-  <si>
     <t>U8</t>
   </si>
   <si>
     <t>LTC3542EDC</t>
   </si>
   <si>
-    <t>DFN-8</t>
+    <t>DFN_6_2X2_SLUG</t>
   </si>
   <si>
     <t>Linear Tech</t>
@@ -741,7 +780,7 @@
     <t>LTC4160</t>
   </si>
   <si>
-    <t>QFN-20</t>
+    <t>QFN20_3X4_WITH_SLUG_0.75H</t>
   </si>
   <si>
     <t>LTC4160EUDC</t>
@@ -765,12 +804,30 @@
     <t>TS3USB221EDRCR</t>
   </si>
   <si>
-    <t>VSON10</t>
+    <t>QFN10_3X3_0.5_SLUG</t>
+  </si>
+  <si>
+    <t>U12</t>
+  </si>
+  <si>
+    <t>LTC2941CDCB</t>
+  </si>
+  <si>
+    <t>DFN_6_2X3_SLUG</t>
+  </si>
+  <si>
+    <t>LTC2941CDCB#TRMPBF</t>
+  </si>
+  <si>
+    <t>LTC2941CDCB#TRMPBFCT-ND</t>
   </si>
   <si>
     <t>VIB1</t>
   </si>
   <si>
+    <t>VIBRO_JINLONG_C1027H300F</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jinlong </t>
   </si>
   <si>
@@ -793,12 +850,6 @@
   </si>
   <si>
     <t>7M-12.000MAAJ-T</t>
-  </si>
-  <si>
-    <t>Bill Of Materials            May 20,2016      12:00:58</t>
-  </si>
-  <si>
-    <t>R33,R39,R50</t>
   </si>
 </sst>
 </file>
@@ -851,7 +902,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SCANNER_revb_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SCANNER_revb" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1141,23 +1192,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I99"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1198,44 +1252,44 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>254</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1246,22 +1300,22 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E15">
         <v>402</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I15">
         <v>1816735</v>
@@ -1269,12 +1323,12 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1285,22 +1339,22 @@
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E18">
         <v>402</v>
       </c>
       <c r="F18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I18">
         <v>2346873</v>
@@ -1308,7 +1362,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1316,25 +1370,25 @@
         <v>3</v>
       </c>
       <c r="B20">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E20">
         <v>402</v>
       </c>
       <c r="F20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I20">
         <v>2210822</v>
@@ -1342,22 +1396,22 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1368,22 +1422,22 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E25">
         <v>402</v>
       </c>
       <c r="F25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H25" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I25">
         <v>2210821</v>
@@ -1397,22 +1451,22 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D26" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E26">
         <v>402</v>
       </c>
       <c r="F26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G26" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H26" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I26">
         <v>2210796</v>
@@ -1426,22 +1480,22 @@
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D27" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E27">
         <v>805</v>
       </c>
       <c r="F27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G27" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I27">
         <v>2309029</v>
@@ -1455,22 +1509,22 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E28">
         <v>805</v>
       </c>
       <c r="F28" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I28">
         <v>1284130</v>
@@ -1484,22 +1538,22 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E29">
         <v>805</v>
       </c>
       <c r="F29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H29" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I29">
         <v>2113069</v>
@@ -1513,22 +1567,22 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E30">
         <v>402</v>
       </c>
       <c r="F30" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G30" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H30" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I30">
         <v>1759375</v>
@@ -1542,22 +1596,22 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D31" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E31" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F31" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G31" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H31" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I31">
         <v>2322105</v>
@@ -1571,22 +1625,22 @@
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F32" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H32" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I32">
         <v>2322113</v>
@@ -1600,22 +1654,22 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E33" t="s">
+        <v>70</v>
+      </c>
+      <c r="F33" t="s">
+        <v>71</v>
+      </c>
+      <c r="G33" t="s">
         <v>69</v>
       </c>
-      <c r="F33" t="s">
-        <v>70</v>
-      </c>
-      <c r="G33" t="s">
-        <v>68</v>
-      </c>
       <c r="H33" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I33">
         <v>1621821</v>
@@ -1629,7 +1683,7 @@
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D34">
         <v>7427927291</v>
@@ -1638,13 +1692,13 @@
         <v>402</v>
       </c>
       <c r="F34" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G34">
         <v>7427927291</v>
       </c>
       <c r="H34" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I34">
         <v>1961694</v>
@@ -1658,22 +1712,22 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D35" t="s">
-        <v>151</v>
+        <v>75</v>
       </c>
       <c r="E35" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F35" t="s">
+        <v>77</v>
+      </c>
+      <c r="G35" t="s">
         <v>76</v>
       </c>
-      <c r="G35" t="s">
-        <v>74</v>
-      </c>
       <c r="H35" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I35" t="s">
         <v>78</v>
@@ -1702,7 +1756,7 @@
         <v>83</v>
       </c>
       <c r="H36" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I36">
         <v>2060699</v>
@@ -1731,7 +1785,7 @@
         <v>1054431101</v>
       </c>
       <c r="H37" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I37">
         <v>2500017</v>
@@ -1760,7 +1814,7 @@
         <v>87</v>
       </c>
       <c r="H38" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I38">
         <v>1125359</v>
@@ -1783,13 +1837,13 @@
         <v>742792651</v>
       </c>
       <c r="F39" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G39">
         <v>742792651</v>
       </c>
       <c r="H39" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I39">
         <v>1635706</v>
@@ -1812,13 +1866,13 @@
         <v>744231091</v>
       </c>
       <c r="F40" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G40">
         <v>744231091</v>
       </c>
       <c r="H40" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I40">
         <v>1636469</v>
@@ -1841,13 +1895,13 @@
         <v>93</v>
       </c>
       <c r="F41" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G41">
         <v>742792651</v>
       </c>
       <c r="H41" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I41">
         <v>1635706</v>
@@ -1866,17 +1920,17 @@
       <c r="D42" t="s">
         <v>95</v>
       </c>
-      <c r="E42">
-        <v>744030003</v>
+      <c r="E42" t="s">
+        <v>96</v>
       </c>
       <c r="F42" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G42">
         <v>744030003</v>
       </c>
       <c r="H42" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I42">
         <v>2211437</v>
@@ -1890,25 +1944,25 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D43" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E43" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F43" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G43" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H43" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I43" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -1919,25 +1973,25 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D44" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E44" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F44" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G44" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H44" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I44" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -1948,22 +2002,22 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D45" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E45" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F45" t="s">
+        <v>114</v>
+      </c>
+      <c r="G45" t="s">
         <v>112</v>
       </c>
-      <c r="G45" t="s">
-        <v>110</v>
-      </c>
       <c r="H45" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I45">
         <v>1791366</v>
@@ -1977,22 +2031,22 @@
         <v>2</v>
       </c>
       <c r="C46" t="s">
+        <v>115</v>
+      </c>
+      <c r="D46" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" t="s">
         <v>113</v>
       </c>
-      <c r="D46" t="s">
-        <v>114</v>
-      </c>
-      <c r="E46" t="s">
-        <v>115</v>
-      </c>
       <c r="F46" t="s">
+        <v>117</v>
+      </c>
+      <c r="G46" t="s">
         <v>116</v>
       </c>
-      <c r="G46" t="s">
-        <v>114</v>
-      </c>
       <c r="H46" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I46">
         <v>8734771</v>
@@ -2006,25 +2060,25 @@
         <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D47" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E47" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F47" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="G47" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="H47" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I47">
-        <v>1081234</v>
+        <v>2317633</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2035,778 +2089,745 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D48" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E48">
         <v>603</v>
       </c>
       <c r="F48" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G48" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="H48" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I48">
         <v>9233156</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>28</v>
       </c>
       <c r="B49">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="C49" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D49" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E49">
         <v>402</v>
       </c>
       <c r="F49" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G49" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H49" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I49">
+        <v>1358096</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>29</v>
+      </c>
+      <c r="B51">
+        <v>25</v>
+      </c>
+      <c r="C51" t="s">
+        <v>131</v>
+      </c>
+      <c r="D51" t="s">
+        <v>132</v>
+      </c>
+      <c r="E51">
+        <v>402</v>
+      </c>
+      <c r="F51" t="s">
+        <v>128</v>
+      </c>
+      <c r="G51" t="s">
+        <v>133</v>
+      </c>
+      <c r="H51" t="s">
+        <v>23</v>
+      </c>
+      <c r="I51">
         <v>1358069</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>30</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>138</v>
+      </c>
+      <c r="D56" t="s">
+        <v>139</v>
+      </c>
+      <c r="E56">
+        <v>402</v>
+      </c>
+      <c r="F56" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>29</v>
-      </c>
-      <c r="B55">
-        <v>11</v>
-      </c>
-      <c r="C55" t="s">
-        <v>132</v>
-      </c>
-      <c r="D55" t="s">
-        <v>133</v>
-      </c>
-      <c r="E55">
-        <v>402</v>
-      </c>
-      <c r="F55" t="s">
-        <v>125</v>
-      </c>
-      <c r="G55" t="s">
-        <v>134</v>
-      </c>
-      <c r="H55" t="s">
-        <v>22</v>
-      </c>
-      <c r="I55">
-        <v>1358096</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
+        <v>140</v>
+      </c>
+      <c r="H56" t="s">
+        <v>23</v>
+      </c>
+      <c r="I56">
+        <v>1358051</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D57" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="E57">
         <v>402</v>
       </c>
       <c r="F57" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G57" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="H57" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I57">
-        <v>1358051</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1358071</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C58" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D58" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="E58">
         <v>402</v>
       </c>
       <c r="F58" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G58" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="H58" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I58">
-        <v>1358071</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1358047</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D59" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="E59">
         <v>402</v>
       </c>
       <c r="F59" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G59" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="H59" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I59">
-        <v>1358047</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1357998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B60">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D60" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E60">
-        <v>402</v>
+        <v>603</v>
       </c>
       <c r="F60" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="G60" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="H60" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I60">
-        <v>1357998</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2112794</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B61">
         <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="D61" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E61">
         <v>402</v>
       </c>
       <c r="F61" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G61" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="H61" t="s">
-        <v>22</v>
-      </c>
-      <c r="I61">
+        <v>23</v>
+      </c>
+      <c r="J61">
         <v>1358073</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B62">
         <v>3</v>
       </c>
       <c r="C62" t="s">
-        <v>255</v>
+        <v>157</v>
       </c>
       <c r="D62" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="E62">
         <v>402</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B63">
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="D63" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="E63">
         <v>805</v>
       </c>
       <c r="F63" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="G63" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="H63" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I63">
         <v>1506149</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B64">
         <v>2</v>
       </c>
       <c r="C64" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="D64" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="E64">
         <v>402</v>
       </c>
       <c r="F64" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G64" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="H64" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I64">
         <v>1803798</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B65">
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="D65" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="E65">
         <v>402</v>
       </c>
       <c r="F65" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G65" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="H65" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I65">
         <v>1358093</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B66">
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="D66" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="E66">
         <v>402</v>
       </c>
       <c r="F66" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G66" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="H66" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I66">
         <v>1358063</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B67">
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="D67" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E67">
         <v>402</v>
       </c>
       <c r="F67" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G67" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="H67" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I67">
         <v>1358123</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B68">
         <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="D68" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="E68">
         <v>402</v>
       </c>
       <c r="F68" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G68" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="H68" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I68">
         <v>2130392</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B69">
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="D69" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="E69">
         <v>402</v>
       </c>
       <c r="F69" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G69" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="H69" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I69">
         <v>1358050</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B70">
         <v>12</v>
       </c>
       <c r="C70" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="D70" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="E70">
         <v>603</v>
       </c>
       <c r="F70" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G70" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="H70" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I70">
         <v>9331387</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B72">
         <v>2</v>
       </c>
       <c r="C72" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="D72" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="E72">
         <v>402</v>
       </c>
       <c r="F72" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G72" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="H72" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I72">
         <v>1358034</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B73">
         <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="D73" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="E73">
         <v>402</v>
       </c>
       <c r="F73" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G73" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="H73" t="s">
-        <v>22</v>
-      </c>
-      <c r="I73">
+        <v>23</v>
+      </c>
+      <c r="J73">
         <v>2130474</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B74">
         <v>1</v>
       </c>
       <c r="C74" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="D74" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="E74" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="F74" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H74" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B75">
         <v>2</v>
       </c>
       <c r="C75" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="D75" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="E75" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="F75" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="G75" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="H75" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I75">
         <v>2056845</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B76">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C76" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="D76" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="E76" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>50</v>
+      </c>
+      <c r="B86">
+        <v>17</v>
+      </c>
       <c r="C86" t="s">
-        <v>200</v>
+        <v>209</v>
+      </c>
+      <c r="D86" t="s">
+        <v>210</v>
+      </c>
+      <c r="E86" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>49</v>
-      </c>
-      <c r="B87">
-        <v>1</v>
-      </c>
       <c r="C87" t="s">
-        <v>201</v>
-      </c>
-      <c r="D87" t="s">
-        <v>202</v>
-      </c>
-      <c r="F87" t="s">
-        <v>203</v>
-      </c>
-      <c r="G87" t="s">
-        <v>202</v>
-      </c>
-      <c r="H87" t="s">
-        <v>204</v>
-      </c>
-      <c r="I87" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>50</v>
-      </c>
-      <c r="B88">
-        <v>1</v>
-      </c>
       <c r="C88" t="s">
-        <v>205</v>
-      </c>
-      <c r="D88" t="s">
-        <v>206</v>
-      </c>
-      <c r="E88" t="s">
-        <v>207</v>
-      </c>
-      <c r="F88" t="s">
-        <v>116</v>
-      </c>
-      <c r="G88" t="s">
-        <v>208</v>
-      </c>
-      <c r="H88" t="s">
-        <v>209</v>
-      </c>
-      <c r="I88" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>51</v>
-      </c>
-      <c r="B89">
-        <v>1</v>
-      </c>
       <c r="C89" t="s">
-        <v>211</v>
-      </c>
-      <c r="D89" t="s">
-        <v>212</v>
-      </c>
-      <c r="E89" t="s">
-        <v>213</v>
-      </c>
-      <c r="F89" t="s">
         <v>214</v>
-      </c>
-      <c r="G89" t="s">
-        <v>212</v>
-      </c>
-      <c r="H89" t="s">
-        <v>22</v>
-      </c>
-      <c r="I89">
-        <v>8690413</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -2827,269 +2848,389 @@
         <v>216</v>
       </c>
       <c r="H90" t="s">
-        <v>22</v>
-      </c>
-      <c r="I90">
-        <v>2136671</v>
+        <v>219</v>
+      </c>
+      <c r="I90" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B91">
         <v>1</v>
       </c>
       <c r="C91" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D91" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E91" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F91" t="s">
-        <v>222</v>
+        <v>117</v>
       </c>
       <c r="G91" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="H91" t="s">
-        <v>22</v>
-      </c>
-      <c r="I91">
-        <v>2295725</v>
+        <v>224</v>
+      </c>
+      <c r="I91" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B92">
         <v>1</v>
       </c>
       <c r="C92" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D92" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="E92" t="s">
-        <v>225</v>
+        <v>113</v>
       </c>
       <c r="F92" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="G92" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="H92" t="s">
-        <v>100</v>
-      </c>
-      <c r="I92" t="s">
-        <v>227</v>
+        <v>23</v>
+      </c>
+      <c r="I92">
+        <v>8690413</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B93">
         <v>1</v>
       </c>
       <c r="C93" t="s">
-        <v>228</v>
-      </c>
-      <c r="D93">
-        <v>82400102</v>
+        <v>229</v>
+      </c>
+      <c r="D93" t="s">
+        <v>230</v>
       </c>
       <c r="E93" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="F93" t="s">
-        <v>72</v>
-      </c>
-      <c r="G93">
-        <v>82400102</v>
+        <v>232</v>
+      </c>
+      <c r="G93" t="s">
+        <v>230</v>
       </c>
       <c r="H93" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I93">
-        <v>1825875</v>
+        <v>2136671</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B94">
         <v>1</v>
       </c>
       <c r="C94" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D94" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E94" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="F94" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G94" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="H94" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I94">
-        <v>1715237</v>
+        <v>2295725</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B95">
         <v>1</v>
       </c>
       <c r="C95" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="D95" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="E95" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F95" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="G95" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H95" t="s">
-        <v>209</v>
+        <v>102</v>
       </c>
       <c r="I95" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B96">
         <v>1</v>
       </c>
       <c r="C96" t="s">
-        <v>239</v>
-      </c>
-      <c r="D96" t="s">
-        <v>240</v>
+        <v>242</v>
+      </c>
+      <c r="D96">
+        <v>82400102</v>
       </c>
       <c r="E96" t="s">
-        <v>241</v>
+        <v>106</v>
       </c>
       <c r="F96" t="s">
-        <v>222</v>
-      </c>
-      <c r="G96" t="s">
-        <v>240</v>
+        <v>73</v>
+      </c>
+      <c r="G96">
+        <v>82400102</v>
       </c>
       <c r="H96" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I96">
-        <v>1105928</v>
+        <v>1825875</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B97">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C97" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D97" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E97" t="s">
+        <v>245</v>
+      </c>
+      <c r="F97" t="s">
+        <v>246</v>
+      </c>
+      <c r="G97" t="s">
         <v>244</v>
       </c>
-      <c r="F97" t="s">
-        <v>222</v>
-      </c>
-      <c r="G97" t="s">
-        <v>243</v>
-      </c>
       <c r="H97" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I97">
-        <v>2383155</v>
+        <v>1715237</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B98">
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D98" t="s">
-        <v>151</v>
+        <v>248</v>
+      </c>
+      <c r="E98" t="s">
+        <v>249</v>
       </c>
       <c r="F98" t="s">
         <v>246</v>
       </c>
       <c r="G98" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="H98" t="s">
-        <v>248</v>
+        <v>224</v>
+      </c>
+      <c r="I98" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B99">
         <v>1</v>
       </c>
       <c r="C99" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D99" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="E99" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="F99" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="G99" t="s">
         <v>253</v>
       </c>
       <c r="H99" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I99">
+        <v>1105928</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>61</v>
+      </c>
+      <c r="B100">
+        <v>2</v>
+      </c>
+      <c r="C100" t="s">
+        <v>255</v>
+      </c>
+      <c r="D100" t="s">
+        <v>256</v>
+      </c>
+      <c r="E100" t="s">
+        <v>257</v>
+      </c>
+      <c r="F100" t="s">
+        <v>236</v>
+      </c>
+      <c r="G100" t="s">
+        <v>256</v>
+      </c>
+      <c r="H100" t="s">
+        <v>23</v>
+      </c>
+      <c r="I100">
+        <v>2383155</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>62</v>
+      </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+      <c r="C101" t="s">
+        <v>258</v>
+      </c>
+      <c r="D101" t="s">
+        <v>259</v>
+      </c>
+      <c r="E101" t="s">
+        <v>260</v>
+      </c>
+      <c r="F101" t="s">
+        <v>246</v>
+      </c>
+      <c r="G101" t="s">
+        <v>261</v>
+      </c>
+      <c r="H101" t="s">
+        <v>224</v>
+      </c>
+      <c r="I101" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>63</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102" t="s">
+        <v>263</v>
+      </c>
+      <c r="D102" t="s">
+        <v>158</v>
+      </c>
+      <c r="E102" t="s">
+        <v>264</v>
+      </c>
+      <c r="F102" t="s">
+        <v>265</v>
+      </c>
+      <c r="G102" t="s">
+        <v>266</v>
+      </c>
+      <c r="H102" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>64</v>
+      </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
+      <c r="C103" t="s">
+        <v>268</v>
+      </c>
+      <c r="D103" t="s">
+        <v>269</v>
+      </c>
+      <c r="E103" t="s">
+        <v>270</v>
+      </c>
+      <c r="F103" t="s">
+        <v>271</v>
+      </c>
+      <c r="G103" t="s">
+        <v>272</v>
+      </c>
+      <c r="H103" t="s">
+        <v>23</v>
+      </c>
+      <c r="I103">
         <v>1842056</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="41" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>